<commit_message>
Align WHO Meningococcal, Cholera, and COVID-19 with current WHO policy
- Meningococcal: remove latestRecAge 18-month cap (WHO supports catch-up)
- Cholera: add single-dose series (WHO emergency policy since Oct 2022),
  keep 2-dose as lower-preference alternative, remove 6-week latestRecInt
- COVID-19: convert from universal Standard to Risk-based series per WHO
  SAGE prioritization (healthcare workers, 60+, immunocompromised), raise
  minimum age from 6 months to 12y abs/18y recommended
- Add observation codes 1020-1022 for COVID-19 risk indications

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/cicada_generator/lib/WHO/antigen/COVID-19.xlsx
+++ b/cicada_generator/lib/WHO/antigen/COVID-19.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="40">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
   <si>
-    <t xml:space="preserve">WHO COVID-19 primary series</t>
+    <t xml:space="preserve">WHO COVID-19 high-priority 2-dose series</t>
   </si>
   <si>
     <t xml:space="preserve">Target Disease</t>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Series Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard</t>
+    <t xml:space="preserve">Risk</t>
   </si>
   <si>
     <t xml:space="preserve">Equivalent Series Groups</t>
@@ -44,18 +44,42 @@
     <t xml:space="preserve">Select Patient Series</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
+    <t xml:space="preserve">High Priority</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
+    <t xml:space="preserve">Indication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healthcare worker (1020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient is a healthcare worker with occupational exposure risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Older adult 60+ years (1021)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient is an older adult (60 years or older)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immunocompromised individual (1022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient is immunocompromised</t>
+  </si>
+  <si>
     <t xml:space="preserve">Series Dose</t>
   </si>
   <si>
@@ -65,7 +89,10 @@
     <t xml:space="preserve">Age</t>
   </si>
   <si>
-    <t xml:space="preserve">6 months</t>
+    <t xml:space="preserve">12 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 years</t>
   </si>
   <si>
     <t xml:space="preserve">Preferable Vaccine</t>
@@ -89,13 +116,7 @@
     <t xml:space="preserve">COVID-19, viral vector (J&amp;J) (212)</t>
   </si>
   <si>
-    <t xml:space="preserve">18 years</t>
-  </si>
-  <si>
     <t xml:space="preserve">COVID-19, protein subunit (Novavax) (211)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 years</t>
   </si>
   <si>
     <t xml:space="preserve">Recurring Dose</t>
@@ -419,10 +440,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -447,130 +468,133 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -578,152 +602,185 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>11</v>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>